<commit_message>
more from end of last day
</commit_message>
<xml_diff>
--- a/Background/Gorilla/logbook_missingdatacheck.xlsx
+++ b/Background/Gorilla/logbook_missingdatacheck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso-my.sharepoint.com/personal/stpis0397_uit_no/Documents/LESS-Project-with-RAs-2/Gorilla/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso-my.sharepoint.com/personal/stpis0397_uit_no/Documents/LESS-Project-with-RAs-2/Background/Gorilla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="8_{585AF805-3B91-4721-B802-F91527BE88B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56A91A63-4260-4A15-AD21-52D58A6E8E3D}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="8_{585AF805-3B91-4721-B802-F91527BE88B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B01572-471E-4BB6-83BB-A9B3A231F95F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7720B47F-B0DD-480C-9D4B-DFCF75350CFC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7720B47F-B0DD-480C-9D4B-DFCF75350CFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Session 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="51">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -186,14 +186,17 @@
     <t xml:space="preserve">missing data, which I downloaded separately </t>
   </si>
   <si>
-    <t>* Benennung der files: TaskName_randomiser, for expample ASRT_ASRT</t>
+    <t>How the names of the exported Gorilla files were transcripted into the names we used for the R analysis</t>
+  </si>
+  <si>
+    <t>* Naming the files: TaskName_randomiser, for expample ASRT_ASRT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +233,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -338,6 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,11 +418,51 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>482950</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>165229</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{622314F9-F596-0888-DC28-C7CA714365D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="196850" y="13646150"/>
+          <a:ext cx="6807550" cy="2514729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,28 +782,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7808207-485A-4602-95CE-0C7DB80F366D}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="40.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="11" max="11" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -770,7 +822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>28</v>
@@ -801,7 +853,7 @@
       </c>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -818,7 +870,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -838,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,7 +907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -875,7 +927,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -889,7 +941,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -909,7 +961,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -926,7 +978,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -946,7 +998,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -966,7 +1018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -986,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1006,7 +1058,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1078,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1046,7 +1098,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1066,7 +1118,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1086,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1106,7 +1158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1178,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1146,7 +1198,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1166,7 +1218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1183,7 +1235,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1255,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1223,40 +1275,45 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1282,21 +1339,21 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>28</v>
@@ -1346,7 +1403,7 @@
       </c>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1420,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +1437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1447,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1407,7 +1464,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1474,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1427,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1447,7 +1504,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1457,7 +1514,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1467,7 +1524,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1477,7 +1534,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1487,7 +1544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1497,7 +1554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1574,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1527,7 +1584,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1594,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1547,7 +1604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1557,7 +1614,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1568,7 +1625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1578,7 +1635,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1589,15 +1646,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>39</v>
       </c>

</xml_diff>